<commit_message>
updated roll and grades
</commit_message>
<xml_diff>
--- a/Work Tracking/Grades.xlsx
+++ b/Work Tracking/Grades.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Norco College\CIS 7 - Discrete Structures\grades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncc\CIS7---Discrete-Structures\Work Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,6 +714,9 @@
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -870,6 +873,9 @@
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
       <c r="E26">
         <v>1</v>
       </c>
@@ -882,6 +888,9 @@
         <v>23</v>
       </c>
       <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Lecture 4 and Assignment 6
</commit_message>
<xml_diff>
--- a/Work Tracking/Grades.xlsx
+++ b/Work Tracking/Grades.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncc\CIS7---Discrete-Structures\Work Tracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Norco College\CIS 7 - Discrete Structures\online\CIS7---Discrete-Structures\Work Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Baesu, Benjamin</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>McDonald, Ryan T.</t>
+  </si>
+  <si>
+    <t>Assignment 4</t>
   </si>
 </sst>
 </file>
@@ -537,104 +540,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G34"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" t="s">
-        <v>30</v>
+      <c r="A2" s="1">
+        <v>2510759</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
+        <v>2314019</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>2513919</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>1910427</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>2304318</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>2518161</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>2445585</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>2605599</v>
+        <v>2249735</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -645,191 +674,217 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
+        <v>2445585</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>2605599</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>2259358</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
         <v>2420156</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>2445577</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
         <v>2657949</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>2559201</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
         <v>2570793</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>2276988</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
         <v>2544498</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>2436031</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>2301160</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>2575265</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>2638532</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>16</v>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>2601097</v>
+        <v>2436031</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>2487675</v>
+        <v>2301160</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
-        <v>2519521</v>
+        <v>2575265</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -843,35 +898,38 @@
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>2252531</v>
+        <v>2638532</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <v>2577494</v>
+        <v>2601097</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>2545999</v>
+        <v>2487675</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -882,104 +940,115 @@
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
+        <v>2519521</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>2702737</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>2252531</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>2577494</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>2545999</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
         <v>2531635</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>2510759</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>2249735</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
         <v>2138056</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <v>2702737</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>2314019</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34">
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="F33">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:G33">
+    <sortCondition ref="B2:B33"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add lecture 5.  Update work tracker
</commit_message>
<xml_diff>
--- a/Work Tracking/Grades.xlsx
+++ b/Work Tracking/Grades.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Norco College\CIS 7 - Discrete Structures\online\CIS7---Discrete-Structures\Work Tracking\"/>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Baesu, Benjamin</t>
   </si>
@@ -141,13 +141,16 @@
   </si>
   <si>
     <t>Assignment 4</t>
+  </si>
+  <si>
+    <t>DROP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +169,21 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -215,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -224,6 +242,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -543,7 +568,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,6 +609,9 @@
       <c r="F2">
         <v>1</v>
       </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -635,7 +663,7 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -646,15 +674,21 @@
       <c r="F6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>2518161</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D7">
+      <c r="C7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="5">
         <v>1</v>
       </c>
     </row>
@@ -703,21 +737,24 @@
       <c r="F10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>2605599</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5">
         <v>1</v>
       </c>
     </row>
@@ -745,7 +782,13 @@
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
       <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="F13">
         <v>1</v>
       </c>
     </row>
@@ -760,6 +803,9 @@
         <v>1</v>
       </c>
       <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
         <v>1</v>
       </c>
     </row>
@@ -791,14 +837,23 @@
       <c r="E16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2559201</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
       <c r="D17">
         <v>1</v>
       </c>
@@ -808,8 +863,11 @@
       <c r="F17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>2570793</v>
       </c>
@@ -823,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2276988</v>
       </c>
@@ -839,8 +897,11 @@
       <c r="F19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>2544498</v>
       </c>
@@ -854,7 +915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>2436031</v>
       </c>
@@ -862,7 +923,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2301160</v>
       </c>
@@ -878,8 +939,11 @@
       <c r="F22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>2575265</v>
       </c>
@@ -895,8 +959,11 @@
       <c r="F23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2638532</v>
       </c>
@@ -904,7 +971,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>2601097</v>
       </c>
@@ -921,7 +988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>2487675</v>
       </c>
@@ -929,7 +996,7 @@
         <v>18</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -937,8 +1004,14 @@
       <c r="E26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>2519521</v>
       </c>
@@ -954,14 +1027,20 @@
       <c r="F27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>2702737</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
       <c r="D28">
         <v>1</v>
       </c>
@@ -971,16 +1050,25 @@
       <c r="F28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2252531</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>2577494</v>
       </c>
@@ -997,21 +1085,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
+    <row r="31" spans="1:7" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6">
         <v>2545999</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="5">
+        <v>1</v>
+      </c>
+      <c r="E31" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>2531635</v>
       </c>
@@ -1027,8 +1115,11 @@
       <c r="F32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>2138056</v>
       </c>
@@ -1036,12 +1127,15 @@
         <v>26</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update lecture 7.  Add Assignment 9
</commit_message>
<xml_diff>
--- a/Work Tracking/Grades.xlsx
+++ b/Work Tracking/Grades.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncc\CIS7---Discrete-Structures\Work Tracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Norco College\CIS 7 - Discrete Structures\online\CIS7---Discrete-Structures\Work Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Baesu, Benjamin</t>
   </si>
@@ -144,13 +144,16 @@
   </si>
   <si>
     <t>Assignment 8</t>
+  </si>
+  <si>
+    <t>Assignment 9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +172,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -218,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -229,6 +240,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,57 +555,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L1" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2510759</v>
       </c>
@@ -612,8 +626,14 @@
       <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2314019</v>
       </c>
@@ -629,11 +649,23 @@
       <c r="F3">
         <v>1</v>
       </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
       <c r="I3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2513919</v>
       </c>
@@ -646,8 +678,11 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1910427</v>
       </c>
@@ -664,7 +699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2304318</v>
       </c>
@@ -672,7 +707,7 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -699,7 +734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2249735</v>
       </c>
@@ -718,8 +753,11 @@
       <c r="I7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2445585</v>
       </c>
@@ -736,7 +774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>32</v>
@@ -759,8 +797,11 @@
       <c r="I9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2259358</v>
       </c>
@@ -780,7 +821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>2420156</v>
       </c>
@@ -812,7 +853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2445577</v>
       </c>
@@ -834,8 +875,11 @@
       <c r="I12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>31</v>
@@ -850,7 +894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>2657949</v>
       </c>
@@ -875,8 +919,14 @@
       <c r="I14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2559201</v>
       </c>
@@ -901,18 +951,39 @@
       <c r="H15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>2570793</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
         <v>1</v>
       </c>
     </row>
@@ -938,6 +1009,9 @@
       <c r="H17">
         <v>1</v>
       </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
@@ -961,6 +1035,9 @@
       <c r="I18">
         <v>1</v>
       </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
@@ -1004,6 +1081,12 @@
       <c r="I20">
         <v>1</v>
       </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
@@ -1030,6 +1113,9 @@
       <c r="I21">
         <v>1</v>
       </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -1070,6 +1156,9 @@
       <c r="J23">
         <v>1</v>
       </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
@@ -1131,6 +1220,12 @@
       <c r="I25">
         <v>1</v>
       </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
@@ -1160,6 +1255,12 @@
       <c r="I26">
         <v>1</v>
       </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
@@ -1186,6 +1287,12 @@
       <c r="I27">
         <v>1</v>
       </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
@@ -1271,6 +1378,9 @@
         <v>1</v>
       </c>
       <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="K30">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add assignment 11.  Update work tracking
</commit_message>
<xml_diff>
--- a/Work Tracking/Grades.xlsx
+++ b/Work Tracking/Grades.xlsx
@@ -571,7 +571,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,6 +1011,9 @@
       <c r="L14">
         <v>1</v>
       </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">

</xml_diff>